<commit_message>
Added changes for Use case1
</commit_message>
<xml_diff>
--- a/myQfcProject/mycommon/target/classes/success.xlsx
+++ b/myQfcProject/mycommon/target/classes/success.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>userid</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Sidd</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,8 +512,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
+      <c r="A8" t="s">
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
@@ -554,6 +557,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>